<commit_message>
Ajout page explication serious game
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorian/Desktop/Master/TP_ConduiteDeProjet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dorian/Desktop/Master/Semestre 2/TP_ConduiteDeProjet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18229C-F3E5-5A49-A323-1E05EEE886D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBC0FA1-8C6E-D744-BEBD-A32125A89995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" xr2:uid="{92EC5B00-75A3-3C4A-9721-E0FC769A85E2}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16320" activeTab="1" xr2:uid="{92EC5B00-75A3-3C4A-9721-E0FC769A85E2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,18 @@
     <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sprint 1'!$B$28</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sprint 1'!$B$29:$B$37</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sprint 1'!$C$28</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sprint 1'!$C$29:$C$37</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sprint 1'!$D$28</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sprint 1'!$D$29:$D$37</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">'Sprint 1'!$D$28</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">'Sprint 1'!$D$29:$D$37</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">'Sprint 1'!$B$28</definedName>
-    <definedName name="_xlchart.v2.7" hidden="1">'Sprint 1'!$B$29:$B$37</definedName>
-    <definedName name="_xlchart.v2.8" hidden="1">'Sprint 1'!$C$28</definedName>
-    <definedName name="_xlchart.v2.9" hidden="1">'Sprint 1'!$C$29:$C$37</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Sprint 2'!$C$24</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Sprint 2'!$C$25:$C$33</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Sprint 2'!$A$24</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Sprint 2'!$A$25:$A$33</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Sprint 2'!$B$24</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Sprint 2'!$B$25:$B$33</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'Sprint 2'!$A$24</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'Sprint 2'!$A$25:$A$33</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'Sprint 2'!$B$24</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'Sprint 2'!$B$25:$B$33</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">'Sprint 2'!$C$24</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">'Sprint 2'!$C$25:$C$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,8 +114,51 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>stakeholdermap.com</author>
+  </authors>
+  <commentList>
+    <comment ref="E38" authorId="0" shapeId="0" xr:uid="{15DA2C39-BA7F-9F4B-BD5C-7FA73877D2F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>stakeholdermap.com:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Number of features or story points actually remaining at the end of each day/iteration/sprint.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -154,6 +197,9 @@
   </si>
   <si>
     <t>Spritn</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
   </si>
 </sst>
 </file>
@@ -249,7 +295,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -272,11 +318,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -318,6 +384,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1578,6 +1653,1006 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>BurnUp Value Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$B$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Valeur</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$A$36:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$36:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0E61-AA45-978A-B2303503243C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Valeur max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$A$36:$A$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$C$36:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0E61-AA45-978A-B2303503243C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2027273359"/>
+        <c:axId val="2027275007"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2027273359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2027275007"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2027275007"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2027273359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>BurnDown Chart Sprint 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$B$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pratique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$A$25:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$B$25:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4723-9B4A-9DA4-2A4924152273}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2'!$C$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Théorique</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2'!$A$25:$A$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2'!$C$25:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.625</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.875</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4723-9B4A-9DA4-2A4924152273}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2087805631"/>
+        <c:axId val="2087855327"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2087805631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2087855327"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2087855327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2087805631"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1658,6 +2733,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -2650,12 +3805,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2672,6 +4867,18 @@
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3132,7 +5339,7 @@
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2464BC0B-AF9E-0A4A-9A1E-85B091FCDFD8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3150,6 +5357,1043 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>12700</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2049" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2049"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5678404C-9219-BC49-A7DB-A7271912E757}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>635000</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2050" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83A6EF4F-D127-FF47-B71C-BCA39FEE9ED9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>635000</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2051" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2051"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB7A47CF-6F3F-7149-969A-3F8529659BE3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>635000</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2052" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2052"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B32B3333-3416-7442-A0E4-E62073490477}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>635000</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2053" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2053"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D254ECDB-3DFD-3F46-8310-AAF3AEB3A11E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>635000</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2054" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2054"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D95E161D-1093-FA48-B194-B2D79E572004}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2057" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2057"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4909C3E0-9C0E-394C-9A2C-84C490F45E1B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2058" name="Check Box 10" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F349B74-587F-CE4E-8BAB-DEF992972F84}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2059" name="Check Box 11" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B55F0922-5523-DD4C-82A6-CF9AD5C7205A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2060" name="Check Box 12" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2060"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C033E93C-3270-2945-9400-72D5DD69E5FE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADE8687E-EC61-F943-A792-2743F3A3FA7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2061" name="Check Box 13" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2061"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CF27752-1CE2-304F-A93D-032376C715F1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2062" name="Check Box 14" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2062"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E7D865F-9FD1-BB44-B6FB-EFDED4ED87CF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2063" name="Check Box 15" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2063"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6BD87933-D431-D44C-8E82-8FE815A9F4D2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99FA34F1-0057-B64F-96FB-C612BE0C4224}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2064" name="Check Box 16" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2064"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0CCC4A0-504F-8C48-89C5-B101E0EF0320}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:oneCellAnchor>
+        <xdr:from>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>279400</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>88900</xdr:rowOff>
+        </xdr:from>
+        <xdr:ext cx="355600" cy="431800"/>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2065" name="Check Box 17" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2065"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F40CC28-CDA0-4E48-B78E-335D4CDB79EA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:oneCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -3452,8 +6696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01070291-FFF4-3048-A4A7-40458FD4120D}">
   <dimension ref="A3:O133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView topLeftCell="A111" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3516,7 +6760,7 @@
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
-      <c r="C7" s="20"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="8">
         <v>1</v>
       </c>
@@ -3533,7 +6777,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
-      <c r="C8" s="20"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="8">
         <v>2</v>
       </c>
@@ -3550,7 +6794,7 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
-      <c r="C9" s="20"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="8">
         <v>3</v>
       </c>
@@ -3567,7 +6811,7 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="11"/>
-      <c r="C10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="8">
         <v>4</v>
       </c>
@@ -3584,7 +6828,7 @@
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
-      <c r="C11" s="20"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="8">
         <v>5</v>
       </c>
@@ -3601,7 +6845,7 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="12"/>
-      <c r="C12" s="20"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="9">
         <v>6</v>
       </c>
@@ -4138,14 +7382,889 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC87DEA-1A07-3C4C-8470-2AB99889AA77}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC87DEA-1A07-3C4C-8470-2AB99889AA77}">
+  <dimension ref="A3:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="10">
+        <v>44210</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="11"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="11"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20">
+        <v>2</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20">
+        <v>3</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="11"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20">
+        <v>4</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="11"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20">
+        <v>5</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="12"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
+        <v>6</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C13" s="23"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9">
+        <v>7</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C14" s="23"/>
+      <c r="D14" s="9">
+        <v>8</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C15" s="23"/>
+      <c r="D15" s="9">
+        <v>9</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="16"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C16" s="23"/>
+      <c r="D16" s="9">
+        <v>10</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="23"/>
+      <c r="D17" s="9">
+        <v>11</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="23"/>
+      <c r="D18" s="9">
+        <v>12</v>
+      </c>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="23"/>
+      <c r="D19" s="9">
+        <v>13</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="23"/>
+      <c r="D20" s="9">
+        <v>14</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="23"/>
+      <c r="D21" s="9">
+        <v>15</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>0</v>
+      </c>
+      <c r="B25" s="4">
+        <v>15</v>
+      </c>
+      <c r="C25" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4">
+        <v>15</v>
+      </c>
+      <c r="C26" s="4">
+        <f>C25-(15/8)</f>
+        <v>13.125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>30</v>
+      </c>
+      <c r="B27" s="4">
+        <v>12</v>
+      </c>
+      <c r="C27" s="4">
+        <f t="shared" ref="C27:C33" si="0">C26-(15/8)</f>
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>45</v>
+      </c>
+      <c r="B28" s="4">
+        <v>10</v>
+      </c>
+      <c r="C28" s="4">
+        <f t="shared" si="0"/>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>60</v>
+      </c>
+      <c r="B29" s="4">
+        <v>9</v>
+      </c>
+      <c r="C29" s="4">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>75</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4">
+        <f t="shared" si="0"/>
+        <v>5.625</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>90</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>105</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4">
+        <f t="shared" si="0"/>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>120</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>0</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>15</v>
+      </c>
+      <c r="B37" s="4">
+        <v>0</v>
+      </c>
+      <c r="C37" s="4">
+        <v>15</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>30</v>
+      </c>
+      <c r="B38" s="4">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4">
+        <v>15</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>45</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5</v>
+      </c>
+      <c r="C39" s="4">
+        <v>15</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>60</v>
+      </c>
+      <c r="B40" s="4">
+        <v>6</v>
+      </c>
+      <c r="C40" s="4">
+        <v>15</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>75</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4">
+        <v>15</v>
+      </c>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>90</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4">
+        <v>15</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>105</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4">
+        <v>15</v>
+      </c>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>120</v>
+      </c>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4">
+        <v>15</v>
+      </c>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="18"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:C21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2049" r:id="rId3" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>12700</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2050" r:id="rId4" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2051" r:id="rId5" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>7</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2052" r:id="rId6" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2053" r:id="rId7" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2054" r:id="rId8" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2057" r:id="rId9" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2058" r:id="rId10" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2059" r:id="rId11" name="Check Box 11">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>13</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2060" r:id="rId12" name="Check Box 12">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2061" r:id="rId13" name="Check Box 13">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>15</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2062" r:id="rId14" name="Check Box 14">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2063" r:id="rId15" name="Check Box 15">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>17</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2064" r:id="rId16" name="Check Box 16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>18</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>20</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="2065" r:id="rId17" name="Check Box 17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>279400</xdr:colOff>
+                    <xdr:row>19</xdr:row>
+                    <xdr:rowOff>88900</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>635000</xdr:colOff>
+                    <xdr:row>21</xdr:row>
+                    <xdr:rowOff>114300</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
 

</xml_diff>